<commit_message>
finished working with reading excel sheet 6-23-25
</commit_message>
<xml_diff>
--- a/bookPractice/excel through python/data/workbook.xlsx
+++ b/bookPractice/excel through python/data/workbook.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="first_sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="second_sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -340,12 +341,442 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>9</v>
+      </c>
+      <c r="C1">
+        <v>17</v>
+      </c>
+      <c r="D1">
+        <v>25</v>
+      </c>
+      <c r="E1">
+        <v>33</v>
+      </c>
+      <c r="F1">
+        <v>41</v>
+      </c>
+      <c r="G1">
+        <v>49</v>
+      </c>
+      <c r="H1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>34</v>
+      </c>
+      <c r="F2">
+        <v>42</v>
+      </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>27</v>
+      </c>
+      <c r="E3">
+        <v>35</v>
+      </c>
+      <c r="F3">
+        <v>43</v>
+      </c>
+      <c r="G3">
+        <v>51</v>
+      </c>
+      <c r="H3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <v>36</v>
+      </c>
+      <c r="F4">
+        <v>44</v>
+      </c>
+      <c r="G4">
+        <v>52</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>37</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="G5">
+        <v>53</v>
+      </c>
+      <c r="H5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6">
+        <v>38</v>
+      </c>
+      <c r="F6">
+        <v>46</v>
+      </c>
+      <c r="G6">
+        <v>54</v>
+      </c>
+      <c r="H6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>39</v>
+      </c>
+      <c r="F7">
+        <v>47</v>
+      </c>
+      <c r="G7">
+        <v>55</v>
+      </c>
+      <c r="H7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>48</v>
+      </c>
+      <c r="G8">
+        <v>56</v>
+      </c>
+      <c r="H8">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>22</v>
+      </c>
+      <c r="G3">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <v>29</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>31</v>
+      </c>
+      <c r="H4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>37</v>
+      </c>
+      <c r="F5">
+        <v>38</v>
+      </c>
+      <c r="G5">
+        <v>39</v>
+      </c>
+      <c r="H5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>41</v>
+      </c>
+      <c r="B6">
+        <v>42</v>
+      </c>
+      <c r="C6">
+        <v>43</v>
+      </c>
+      <c r="D6">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>46</v>
+      </c>
+      <c r="G6">
+        <v>47</v>
+      </c>
+      <c r="H6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>49</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>51</v>
+      </c>
+      <c r="D7">
+        <v>52</v>
+      </c>
+      <c r="E7">
+        <v>53</v>
+      </c>
+      <c r="F7">
+        <v>54</v>
+      </c>
+      <c r="G7">
+        <v>55</v>
+      </c>
+      <c r="H7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>57</v>
+      </c>
+      <c r="B8">
+        <v>58</v>
+      </c>
+      <c r="C8">
+        <v>59</v>
+      </c>
+      <c r="D8">
+        <v>60</v>
+      </c>
+      <c r="E8">
+        <v>61</v>
+      </c>
+      <c r="F8">
+        <v>62</v>
+      </c>
+      <c r="G8">
+        <v>63</v>
+      </c>
+      <c r="H8">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>